<commit_message>
Latest modifications on DNAUpgrade
</commit_message>
<xml_diff>
--- a/DNA_Upgrade_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/DNA_Upgrade_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\OLB\InstantOpen_Automation\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECUProjects\DNA_Upgrade_Automation\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE6637E-5A70-496F-AE37-6924FE0E5501}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7CCD3F-2594-4D09-BE2D-445CA4592003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -637,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,7 +1172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="U5" sqref="U5"/>
     </sheetView>

</xml_diff>